<commit_message>
CNS figs + KS summary
</commit_message>
<xml_diff>
--- a/patientData/PtDirectorySimple.xlsx
+++ b/patientData/PtDirectorySimple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sydne\Documents\github\perceive\patientData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8661CD39-373A-4992-81D9-CA94BD46E6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBF390B-8D25-4EEB-BFC0-670DA58D0C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="1330" windowWidth="19200" windowHeight="11260" xr2:uid="{20656A42-143D-4896-9146-1E8421386A29}"/>
   </bookViews>
@@ -42,12 +42,6 @@
     <t>Hemisphere</t>
   </si>
   <si>
-    <t>Json Survey</t>
-  </si>
-  <si>
-    <t>Json Stream</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -90,10 +84,16 @@
     <t>pt4_0819_r_stream.json</t>
   </si>
   <si>
-    <t>Start Index</t>
-  </si>
-  <si>
-    <t>Double Battery</t>
+    <t>JsonSurvey</t>
+  </si>
+  <si>
+    <t>JsonStream</t>
+  </si>
+  <si>
+    <t>StartIndex</t>
+  </si>
+  <si>
+    <t>DoubleBattery</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,7 +460,9 @@
     <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="10.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -471,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
@@ -488,13 +490,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>7</v>
@@ -508,13 +510,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
@@ -528,13 +530,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -548,13 +550,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -568,13 +570,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -588,16 +590,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -608,13 +610,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>

</xml_diff>